<commit_message>
add contrasts to sst
</commit_message>
<xml_diff>
--- a/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal_condsonly.xlsx
+++ b/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal_condsonly.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadestasio/Desktop/REV_scripts/fMRI/fx/SST/prepost_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF4D3E56-89E0-AB44-AAF7-714AB9697CD2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7235EA23-3989-FA4B-BBB4-CCA08EB09E29}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F44029D5-836C-9941-B0F2-754275B93E74}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Run 1</t>
   </si>
@@ -86,13 +86,43 @@
     <t>8_T2(AnyStop&gt;CorrectGo)&gt;T1(AnyStop&gt;CorrectGo)</t>
   </si>
   <si>
-    <t>9_T2 (Correct Stop) &gt; T1 (Correct Stop)</t>
+    <t>All runs</t>
   </si>
   <si>
-    <t>10_T2 (Any Stop) &gt; T1 (Any Stop)</t>
+    <t>11_CorrectStop&gt;CorrectGo_pre</t>
   </si>
   <si>
-    <t>All runs</t>
+    <t>12_CorrectStop&gt;IncorrectStop_pre</t>
+  </si>
+  <si>
+    <t>13_AnyStop&gt;Baseline_pre</t>
+  </si>
+  <si>
+    <t>15_AnyStop&gt;CorrectGo_pre</t>
+  </si>
+  <si>
+    <t>14_CorrectGo&gt;Baseline_pre</t>
+  </si>
+  <si>
+    <t>9_T2(Correct Stop)&gt;T1(Correct Stop)</t>
+  </si>
+  <si>
+    <t>10_T2(Any Stop)&gt;T1(Any Stop)</t>
+  </si>
+  <si>
+    <t>16_CorrectStop&gt;CorrectGo_post</t>
+  </si>
+  <si>
+    <t>17_CorrectStop&gt;IncorrectStop_post</t>
+  </si>
+  <si>
+    <t>18_AnyStop&gt;Baseline_post</t>
+  </si>
+  <si>
+    <t>19_CorrectGo&gt;Baseline_post</t>
+  </si>
+  <si>
+    <t>20_AnyStop&gt;CorrectGo_post</t>
   </si>
 </sst>
 </file>
@@ -227,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -253,6 +283,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C102CF70-CBA0-A749-8140-E7CAFBFE284A}">
   <dimension ref="A1:XDP43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:U13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,9 +616,9 @@
     <col min="1" max="1" width="53.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1"/>
       <c r="G1" s="1"/>
@@ -591,7 +629,7 @@
       <c r="T1" s="18"/>
       <c r="U1" s="18"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +647,7 @@
       <c r="T2" s="18"/>
       <c r="U2" s="18"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -674,7 +712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -739,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -804,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -869,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
@@ -934,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -1064,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -1129,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
@@ -1194,9 +1232,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B12" s="24">
         <v>0</v>
@@ -1261,9 +1299,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B13" s="24">
         <v>0</v>
@@ -1326,8 +1364,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
@@ -1338,242 +1378,436 @@
       <c r="I14" s="24"/>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
+      <c r="L14" s="24">
+        <v>0</v>
+      </c>
+      <c r="M14" s="24">
+        <v>0</v>
+      </c>
+      <c r="N14" s="24">
+        <v>0</v>
+      </c>
+      <c r="O14" s="24">
+        <v>0</v>
+      </c>
+      <c r="P14" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="24">
+        <v>0</v>
+      </c>
+      <c r="R14" s="24">
+        <v>0</v>
+      </c>
+      <c r="S14" s="24">
+        <v>0</v>
+      </c>
+      <c r="T14" s="24">
+        <v>0</v>
+      </c>
+      <c r="U14" s="24">
+        <v>0</v>
+      </c>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26">
+        <v>0</v>
+      </c>
+      <c r="M15" s="26">
+        <v>0</v>
+      </c>
+      <c r="N15" s="26">
+        <v>0</v>
+      </c>
+      <c r="O15" s="26">
+        <v>0</v>
+      </c>
+      <c r="P15" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="26">
+        <v>0</v>
+      </c>
+      <c r="R15" s="26">
+        <v>0</v>
+      </c>
+      <c r="S15" s="26">
+        <v>0</v>
+      </c>
+      <c r="T15" s="26">
+        <v>0</v>
+      </c>
+      <c r="U15" s="26">
+        <v>0</v>
+      </c>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26">
+        <v>0</v>
+      </c>
+      <c r="M16" s="26">
+        <v>0</v>
+      </c>
+      <c r="N16" s="26">
+        <v>0</v>
+      </c>
+      <c r="O16" s="26">
+        <v>0</v>
+      </c>
+      <c r="P16" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="26">
+        <v>0</v>
+      </c>
+      <c r="R16" s="26">
+        <v>0</v>
+      </c>
+      <c r="S16" s="26">
+        <v>0</v>
+      </c>
+      <c r="T16" s="26">
+        <v>0</v>
+      </c>
+      <c r="U16" s="26">
+        <v>0</v>
+      </c>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
     </row>
     <row r="17" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
+      <c r="A17" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26">
+        <v>0</v>
+      </c>
+      <c r="M17" s="26">
+        <v>0</v>
+      </c>
+      <c r="N17" s="26">
+        <v>0</v>
+      </c>
+      <c r="O17" s="26">
+        <v>0</v>
+      </c>
+      <c r="P17" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="30">
+        <v>0</v>
+      </c>
+      <c r="R17" s="30">
+        <v>0</v>
+      </c>
+      <c r="S17" s="30">
+        <v>0</v>
+      </c>
+      <c r="T17" s="30">
+        <v>0</v>
+      </c>
+      <c r="U17" s="30">
+        <v>0</v>
+      </c>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
     </row>
     <row r="18" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
+      <c r="A18" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="32">
+        <v>0</v>
+      </c>
+      <c r="M18" s="32">
+        <v>0</v>
+      </c>
+      <c r="N18" s="32">
+        <v>0</v>
+      </c>
+      <c r="O18" s="32">
+        <v>0</v>
+      </c>
+      <c r="P18" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="32">
+        <v>0</v>
+      </c>
+      <c r="R18" s="32">
+        <v>0</v>
+      </c>
+      <c r="S18" s="32">
+        <v>0</v>
+      </c>
+      <c r="T18" s="32">
+        <v>0</v>
+      </c>
+      <c r="U18" s="32">
+        <v>0</v>
+      </c>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
     </row>
     <row r="19" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="7"/>
+      <c r="A19" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
     </row>
     <row r="20" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="10"/>
+      <c r="A20" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
     </row>
     <row r="21" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="12"/>
+      <c r="A21" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
     </row>
     <row r="22" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
+      <c r="A22" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
     </row>
     <row r="23" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="17"/>
+      <c r="A23" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
     </row>
     <row r="24" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="7"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
     </row>
     <row r="25" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="10"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="26"/>
     </row>
     <row r="26" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="22"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
       <c r="X26" s="22"/>
       <c r="Y26" s="22"/>
       <c r="Z26" s="22"/>
@@ -17897,257 +18131,429 @@
       <c r="XDP26" s="22"/>
     </row>
     <row r="27" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="24"/>
-      <c r="U27" s="24"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
     </row>
     <row r="28" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+    </row>
+    <row r="29" spans="1:16344" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+    </row>
+    <row r="30" spans="1:16344" x14ac:dyDescent="0.2">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="22"/>
+      <c r="V30" s="22"/>
+      <c r="W30" s="22"/>
     </row>
     <row r="31" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
+      <c r="V31" s="22"/>
+      <c r="W31" s="22"/>
     </row>
     <row r="32" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A33" s="25"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="7"/>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A34" s="25"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="22"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="22"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="10"/>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A35" s="25"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="12"/>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A36" s="25"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A37" s="25"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="22"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A38" s="25"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="22"/>
+      <c r="V38" s="22"/>
+      <c r="W38" s="22"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="7"/>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A39" s="25"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
+      <c r="U39" s="22"/>
+      <c r="V39" s="22"/>
+      <c r="W39" s="22"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="10"/>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A40" s="25"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="22"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="22"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="21"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A41" s="25"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="22"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
+      <c r="U41" s="22"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="22"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="24"/>
-      <c r="O42" s="24"/>
-      <c r="P42" s="24"/>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A42" s="25"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
+      <c r="U42" s="22"/>
+      <c r="V42" s="22"/>
+      <c r="W42" s="22"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="24"/>
-      <c r="O43" s="24"/>
-      <c r="P43" s="24"/>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A43" s="25"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
+      <c r="U43" s="22"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new contrast T1T2CorrGo
</commit_message>
<xml_diff>
--- a/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal_condsonly.xlsx
+++ b/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal_condsonly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadestasio/Desktop/REV_scripts/fMRI/fx/SST/prepost_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEDF39E-623A-0042-944C-859B55A958A6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6349164-732F-264C-8BAE-F48BD7115F80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F44029D5-836C-9941-B0F2-754275B93E74}"/>
+    <workbookView xWindow="54400" yWindow="0" windowWidth="12800" windowHeight="24000" xr2:uid="{F44029D5-836C-9941-B0F2-754275B93E74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Run 1</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>20_AnyStopTrial&gt;CorrectGo_post</t>
+  </si>
+  <si>
+    <t>21_T2(CorrectGo)&gt;T1(CorrectGo)</t>
   </si>
 </sst>
 </file>
@@ -613,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C102CF70-CBA0-A749-8140-E7CAFBFE284A}">
   <dimension ref="A1:XDP43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2041,27 +2044,69 @@
       <c r="W23" s="35"/>
     </row>
     <row r="24" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="20"/>
+      <c r="A24" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="20">
+        <v>0</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0</v>
+      </c>
+      <c r="E24" s="20">
+        <v>0</v>
+      </c>
+      <c r="F24" s="20">
+        <v>0</v>
+      </c>
+      <c r="G24" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="H24" s="20">
+        <v>0</v>
+      </c>
+      <c r="I24" s="20">
+        <v>0</v>
+      </c>
+      <c r="J24" s="20">
+        <v>0</v>
+      </c>
+      <c r="K24" s="20">
+        <v>0</v>
+      </c>
+      <c r="L24" s="20">
+        <v>-0.5</v>
+      </c>
+      <c r="M24" s="20">
+        <v>0</v>
+      </c>
+      <c r="N24" s="20">
+        <v>0</v>
+      </c>
+      <c r="O24" s="20">
+        <v>0</v>
+      </c>
+      <c r="P24" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="20">
+        <v>-0.5</v>
+      </c>
+      <c r="R24" s="20">
+        <v>0</v>
+      </c>
+      <c r="S24" s="20">
+        <v>0</v>
+      </c>
+      <c r="T24" s="20">
+        <v>0</v>
+      </c>
+      <c r="U24" s="20">
+        <v>0</v>
+      </c>
       <c r="V24" s="22"/>
       <c r="W24" s="22"/>
     </row>

</xml_diff>

<commit_message>
add contrasts for correctStop vs baseline at T1 and T2
</commit_message>
<xml_diff>
--- a/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal_condsonly.xlsx
+++ b/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal_condsonly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadestasio/Desktop/REV_scripts/fMRI/fx/SST/prepost_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6349164-732F-264C-8BAE-F48BD7115F80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F3A11A-0234-8C41-A38B-5058CF807BBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54400" yWindow="0" windowWidth="12800" windowHeight="24000" xr2:uid="{F44029D5-836C-9941-B0F2-754275B93E74}"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{F44029D5-836C-9941-B0F2-754275B93E74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Run 1</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>21_T2(CorrectGo)&gt;T1(CorrectGo)</t>
+  </si>
+  <si>
+    <t>22_CorrectStop&gt;Baseline_pre</t>
+  </si>
+  <si>
+    <t>23_CorrectStop&gt;Baseline_post</t>
   </si>
 </sst>
 </file>
@@ -616,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C102CF70-CBA0-A749-8140-E7CAFBFE284A}">
   <dimension ref="A1:XDP43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2111,52 +2117,136 @@
       <c r="W24" s="22"/>
     </row>
     <row r="25" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="20"/>
-      <c r="U25" s="20"/>
+      <c r="A25" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="20">
+        <v>0</v>
+      </c>
+      <c r="C25" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="20">
+        <v>0</v>
+      </c>
+      <c r="E25" s="20">
+        <v>0</v>
+      </c>
+      <c r="F25" s="20">
+        <v>0</v>
+      </c>
+      <c r="G25" s="20">
+        <v>0</v>
+      </c>
+      <c r="H25" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="20">
+        <v>0</v>
+      </c>
+      <c r="J25" s="20">
+        <v>0</v>
+      </c>
+      <c r="K25" s="20">
+        <v>0</v>
+      </c>
+      <c r="L25" s="20">
+        <v>0</v>
+      </c>
+      <c r="M25" s="20">
+        <v>0</v>
+      </c>
+      <c r="N25" s="20">
+        <v>0</v>
+      </c>
+      <c r="O25" s="20">
+        <v>0</v>
+      </c>
+      <c r="P25" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="20">
+        <v>0</v>
+      </c>
+      <c r="R25" s="20">
+        <v>0</v>
+      </c>
+      <c r="S25" s="20">
+        <v>0</v>
+      </c>
+      <c r="T25" s="20">
+        <v>0</v>
+      </c>
+      <c r="U25" s="20">
+        <v>0</v>
+      </c>
       <c r="V25" s="22"/>
       <c r="W25" s="22"/>
     </row>
     <row r="26" spans="1:16344" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20"/>
-      <c r="U26" s="20"/>
+      <c r="A26" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="20">
+        <v>0</v>
+      </c>
+      <c r="C26" s="20">
+        <v>0</v>
+      </c>
+      <c r="D26" s="20">
+        <v>0</v>
+      </c>
+      <c r="E26" s="20">
+        <v>0</v>
+      </c>
+      <c r="F26" s="20">
+        <v>0</v>
+      </c>
+      <c r="G26" s="20">
+        <v>0</v>
+      </c>
+      <c r="H26" s="20">
+        <v>0</v>
+      </c>
+      <c r="I26" s="20">
+        <v>0</v>
+      </c>
+      <c r="J26" s="20">
+        <v>0</v>
+      </c>
+      <c r="K26" s="20">
+        <v>0</v>
+      </c>
+      <c r="L26" s="20">
+        <v>0</v>
+      </c>
+      <c r="M26" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="N26" s="20">
+        <v>0</v>
+      </c>
+      <c r="O26" s="20">
+        <v>0</v>
+      </c>
+      <c r="P26" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="20">
+        <v>0</v>
+      </c>
+      <c r="R26" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="S26" s="20">
+        <v>0</v>
+      </c>
+      <c r="T26" s="20">
+        <v>0</v>
+      </c>
+      <c r="U26" s="20">
+        <v>0</v>
+      </c>
       <c r="V26" s="22"/>
       <c r="W26" s="22"/>
       <c r="X26" s="19"/>

</xml_diff>